<commit_message>
GBP_YC bootstrap - fix triggers
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/GBP_YCBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/GBP_YCBootstrapping.xlsx
@@ -28,7 +28,7 @@
     <definedName name="IborType">'General Settings'!$D$7</definedName>
     <definedName name="IndexTenor">'General Settings'!$D$6</definedName>
     <definedName name="InterpolatorID">'General Settings'!$D$25</definedName>
-    <definedName name="MinDistance">RateHelpers!$J$2:$J$122</definedName>
+    <definedName name="MinDistance">RateHelpers!$J$2:$J$104</definedName>
     <definedName name="MoneyMarketDayCounter">'General Settings'!$M$13</definedName>
     <definedName name="Months">'General Settings'!$D$5</definedName>
     <definedName name="NDays">'General Settings'!$D$17</definedName>
@@ -39,9 +39,9 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Selected!$D$1:$J$50</definedName>
     <definedName name="QuoteSuffix">'General Settings'!$M$14</definedName>
     <definedName name="RateHelperPrefix">'General Settings'!$D$9</definedName>
-    <definedName name="RateHelpers">RateHelpers!$E$2:$E$122</definedName>
-    <definedName name="RateHelpersIncluded">RateHelpers!$H$2:$H$122</definedName>
-    <definedName name="RateHelpersPriority">RateHelpers!$I$2:$I$122</definedName>
+    <definedName name="RateHelpers">RateHelpers!$E$2:$E$104</definedName>
+    <definedName name="RateHelpersIncluded">RateHelpers!$H$2:$H$104</definedName>
+    <definedName name="RateHelpersPriority">RateHelpers!$I$2:$I$104</definedName>
     <definedName name="RateHelpersSelected">Selected!$A$7</definedName>
     <definedName name="SerializationPath">'General Settings'!$M$5</definedName>
     <definedName name="Serialize">'General Settings'!$M$4</definedName>
@@ -215,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="176">
   <si>
     <t>60Y</t>
   </si>
@@ -1703,21 +1703,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1738,6 +1723,21 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2056,39 +2056,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="146" customWidth="1"/>
-    <col min="3" max="3" width="18" style="146" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="146" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="146" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2.7109375" style="146" customWidth="1"/>
-    <col min="8" max="9" width="8" style="146"/>
-    <col min="10" max="11" width="2.7109375" style="146" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="146" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53.7109375" style="146" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" style="146" customWidth="1"/>
-    <col min="15" max="16384" width="8" style="146"/>
+    <col min="1" max="2" width="2.7109375" style="141" customWidth="1"/>
+    <col min="3" max="3" width="18" style="141" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="141" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="141" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2.7109375" style="141" customWidth="1"/>
+    <col min="8" max="9" width="8" style="141"/>
+    <col min="10" max="11" width="2.7109375" style="141" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="141" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.7109375" style="141" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="141" customWidth="1"/>
+    <col min="15" max="16384" width="8" style="141"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="146" t="str">
+      <c r="B1" s="141" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
         <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Dec  5 2013 11:03:51</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="149" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="156"/>
-      <c r="K2" s="154" t="s">
+      <c r="C2" s="150"/>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150"/>
+      <c r="F2" s="151"/>
+      <c r="K2" s="149" t="s">
         <v>174</v>
       </c>
-      <c r="L2" s="155"/>
-      <c r="M2" s="155"/>
-      <c r="N2" s="157"/>
+      <c r="L2" s="150"/>
+      <c r="M2" s="150"/>
+      <c r="N2" s="152"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="61"/>
@@ -2111,10 +2111,10 @@
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="57"/>
-      <c r="H4" s="149" t="s">
+      <c r="H4" s="144" t="s">
         <v>117</v>
       </c>
-      <c r="I4" s="150"/>
+      <c r="I4" s="145"/>
       <c r="K4" s="136"/>
       <c r="L4" s="135" t="s">
         <v>173</v>
@@ -2132,10 +2132,10 @@
       <c r="D5" s="62"/>
       <c r="E5" s="58"/>
       <c r="F5" s="57"/>
-      <c r="H5" s="147" t="s">
+      <c r="H5" s="142" t="s">
         <v>115</v>
       </c>
-      <c r="I5" s="148" t="s">
+      <c r="I5" s="143" t="s">
         <v>114</v>
       </c>
       <c r="K5" s="136"/>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="62"/>
       <c r="E6" s="58"/>
       <c r="F6" s="57"/>
-      <c r="H6" s="147" t="s">
+      <c r="H6" s="142" t="s">
         <v>112</v>
       </c>
-      <c r="I6" s="148"/>
+      <c r="I6" s="143"/>
       <c r="K6" s="136"/>
       <c r="L6" s="135" t="s">
         <v>171</v>
@@ -2179,10 +2179,10 @@
       </c>
       <c r="E7" s="58"/>
       <c r="F7" s="57"/>
-      <c r="H7" s="147" t="s">
+      <c r="H7" s="142" t="s">
         <v>110</v>
       </c>
-      <c r="I7" s="148"/>
+      <c r="I7" s="143"/>
       <c r="K7" s="133"/>
       <c r="L7" s="132"/>
       <c r="M7" s="132"/>
@@ -2196,16 +2196,16 @@
       <c r="D8" s="62"/>
       <c r="E8" s="58"/>
       <c r="F8" s="57"/>
-      <c r="H8" s="151" t="s">
+      <c r="H8" s="146" t="s">
         <v>108</v>
       </c>
-      <c r="I8" s="152" t="s">
+      <c r="I8" s="147" t="s">
         <v>107</v>
       </c>
-      <c r="K8" s="153"/>
-      <c r="L8" s="153"/>
-      <c r="M8" s="153"/>
-      <c r="N8" s="153"/>
+      <c r="K8" s="148"/>
+      <c r="L8" s="148"/>
+      <c r="M8" s="148"/>
+      <c r="N8" s="148"/>
     </row>
     <row r="9" spans="2:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
@@ -2218,12 +2218,12 @@
       </c>
       <c r="E9" s="58"/>
       <c r="F9" s="57"/>
-      <c r="K9" s="154" t="s">
+      <c r="K9" s="149" t="s">
         <v>170</v>
       </c>
-      <c r="L9" s="155"/>
-      <c r="M9" s="155"/>
-      <c r="N9" s="157"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="150"/>
+      <c r="N9" s="152"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="61"/>
@@ -2246,7 +2246,7 @@
         <v>104</v>
       </c>
       <c r="D11" s="86">
-        <v>41653.029131944444</v>
+        <v>41653.038877314815</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="57"/>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="D14" s="83" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_GBPYC#0006</v>
+        <v>_GBPYC#0000</v>
       </c>
       <c r="E14" s="58"/>
       <c r="F14" s="57"/>
@@ -2560,11 +2560,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:M122"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2583,11 +2581,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="140" t="s">
+      <c r="B1" s="153" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="141"/>
-      <c r="D1" s="142"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="155"/>
       <c r="E1" s="31" t="s">
         <v>78</v>
       </c>
@@ -3626,7 +3624,7 @@
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="21" t="str">
-        <f t="shared" ref="E28:E59" si="2">RateHelperPrefix&amp;"_"&amp;$B28&amp;$C28&amp;$D28</f>
+        <f t="shared" ref="E28:E34" si="2">RateHelperPrefix&amp;"_"&amp;$B28&amp;$C28&amp;$D28</f>
         <v>GBP_YCRH_1S12</v>
       </c>
       <c r="F28" s="20" t="e">
@@ -3892,8 +3890,8 @@
         <v>37</v>
       </c>
       <c r="E35" s="21" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_SWOIS</v>
+        <f>Discount!L6</f>
+        <v>GBP_YCRH_SWOIS#0000</v>
       </c>
       <c r="F35" s="20">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
@@ -3930,8 +3928,8 @@
         <v>37</v>
       </c>
       <c r="E36" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_2WOIS</v>
+        <f>Discount!L7</f>
+        <v>GBP_YCRH_2WOIS#0000</v>
       </c>
       <c r="F36" s="13">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -3968,8 +3966,8 @@
         <v>37</v>
       </c>
       <c r="E37" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_3WOIS</v>
+        <f>Discount!L8</f>
+        <v>GBP_YCRH_3WOIS#0000</v>
       </c>
       <c r="F37" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -4006,8 +4004,8 @@
         <v>37</v>
       </c>
       <c r="E38" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_1MOIS</v>
+        <f>Discount!L9</f>
+        <v>GBP_YCRH_1MOIS#0000</v>
       </c>
       <c r="F38" s="13">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -4044,8 +4042,8 @@
         <v>37</v>
       </c>
       <c r="E39" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_2MOIS</v>
+        <f>Discount!L10</f>
+        <v>GBP_YCRH_2MOIS#0000</v>
       </c>
       <c r="F39" s="13">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4082,8 +4080,8 @@
         <v>37</v>
       </c>
       <c r="E40" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_3MOIS</v>
+        <f>Discount!L11</f>
+        <v>GBP_YCRH_3MOIS#0000</v>
       </c>
       <c r="F40" s="13">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4120,8 +4118,8 @@
         <v>37</v>
       </c>
       <c r="E41" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_4MOIS</v>
+        <f>Discount!L12</f>
+        <v>GBP_YCRH_4MOIS#0000</v>
       </c>
       <c r="F41" s="13">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4158,8 +4156,8 @@
         <v>37</v>
       </c>
       <c r="E42" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_5MOIS</v>
+        <f>Discount!L13</f>
+        <v>GBP_YCRH_5MOIS#0000</v>
       </c>
       <c r="F42" s="13">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4196,8 +4194,8 @@
         <v>37</v>
       </c>
       <c r="E43" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_6MOIS</v>
+        <f>Discount!L14</f>
+        <v>GBP_YCRH_6MOIS#0000</v>
       </c>
       <c r="F43" s="13">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4234,8 +4232,8 @@
         <v>37</v>
       </c>
       <c r="E44" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_7MOIS</v>
+        <f>Discount!L15</f>
+        <v>GBP_YCRH_7MOIS#0000</v>
       </c>
       <c r="F44" s="13">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4272,8 +4270,8 @@
         <v>37</v>
       </c>
       <c r="E45" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_8MOIS</v>
+        <f>Discount!L16</f>
+        <v>GBP_YCRH_8MOIS#0000</v>
       </c>
       <c r="F45" s="13">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4310,8 +4308,8 @@
         <v>37</v>
       </c>
       <c r="E46" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_9MOIS</v>
+        <f>Discount!L17</f>
+        <v>GBP_YCRH_9MOIS#0000</v>
       </c>
       <c r="F46" s="13">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
@@ -4348,8 +4346,8 @@
         <v>37</v>
       </c>
       <c r="E47" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_10MOIS</v>
+        <f>Discount!L18</f>
+        <v>GBP_YCRH_10MOIS#0000</v>
       </c>
       <c r="F47" s="13">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -4386,8 +4384,8 @@
         <v>37</v>
       </c>
       <c r="E48" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_11MOIS</v>
+        <f>Discount!L19</f>
+        <v>GBP_YCRH_11MOIS#0000</v>
       </c>
       <c r="F48" s="13">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
@@ -4424,8 +4422,8 @@
         <v>37</v>
       </c>
       <c r="E49" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_1YOIS</v>
+        <f>Discount!L20</f>
+        <v>GBP_YCRH_1YOIS#0000</v>
       </c>
       <c r="F49" s="13">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
@@ -4462,8 +4460,8 @@
         <v>37</v>
       </c>
       <c r="E50" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_15MOIS</v>
+        <f>Discount!L21</f>
+        <v>GBP_YCRH_15MOIS#0000</v>
       </c>
       <c r="F50" s="13">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
@@ -4500,8 +4498,8 @@
         <v>37</v>
       </c>
       <c r="E51" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_18MOIS</v>
+        <f>Discount!L22</f>
+        <v>GBP_YCRH_18MOIS#0000</v>
       </c>
       <c r="F51" s="13">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
@@ -4538,8 +4536,8 @@
         <v>37</v>
       </c>
       <c r="E52" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_21MOIS</v>
+        <f>Discount!L23</f>
+        <v>GBP_YCRH_21MOIS#0000</v>
       </c>
       <c r="F52" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
@@ -4576,8 +4574,8 @@
         <v>37</v>
       </c>
       <c r="E53" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_2YOIS</v>
+        <f>Discount!L24</f>
+        <v>GBP_YCRH_2YOIS#0000</v>
       </c>
       <c r="F53" s="13">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
@@ -4614,8 +4612,8 @@
         <v>37</v>
       </c>
       <c r="E54" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_3YOIS</v>
+        <f>Discount!L25</f>
+        <v>GBP_YCRH_3YOIS#0000</v>
       </c>
       <c r="F54" s="13">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
@@ -4652,8 +4650,8 @@
         <v>37</v>
       </c>
       <c r="E55" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_4YOIS</v>
+        <f>Discount!L26</f>
+        <v>GBP_YCRH_4YOIS#0000</v>
       </c>
       <c r="F55" s="13">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
@@ -4690,8 +4688,8 @@
         <v>37</v>
       </c>
       <c r="E56" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_5YOIS</v>
+        <f>Discount!L27</f>
+        <v>GBP_YCRH_5YOIS#0000</v>
       </c>
       <c r="F56" s="13">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
@@ -4728,8 +4726,8 @@
         <v>37</v>
       </c>
       <c r="E57" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_6YOIS</v>
+        <f>Discount!L28</f>
+        <v>GBP_YCRH_6YOIS#0000</v>
       </c>
       <c r="F57" s="13">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
@@ -4766,8 +4764,8 @@
         <v>37</v>
       </c>
       <c r="E58" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_7YOIS</v>
+        <f>Discount!L29</f>
+        <v>GBP_YCRH_7YOIS#0000</v>
       </c>
       <c r="F58" s="13">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
@@ -4804,8 +4802,8 @@
         <v>37</v>
       </c>
       <c r="E59" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v>GBP_YCRH_8YOIS</v>
+        <f>Discount!L30</f>
+        <v>GBP_YCRH_8YOIS#0000</v>
       </c>
       <c r="F59" s="13">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
@@ -4842,8 +4840,8 @@
         <v>37</v>
       </c>
       <c r="E60" s="14" t="str">
-        <f t="shared" ref="E60:E91" si="3">RateHelperPrefix&amp;"_"&amp;$B60&amp;$C60&amp;$D60</f>
-        <v>GBP_YCRH_9YOIS</v>
+        <f>Discount!L31</f>
+        <v>GBP_YCRH_9YOIS#0000</v>
       </c>
       <c r="F60" s="13">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
@@ -4880,8 +4878,8 @@
         <v>37</v>
       </c>
       <c r="E61" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_10YOIS</v>
+        <f>Discount!L32</f>
+        <v>GBP_YCRH_10YOIS#0000</v>
       </c>
       <c r="F61" s="13">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
@@ -4918,8 +4916,8 @@
         <v>37</v>
       </c>
       <c r="E62" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_11YOIS</v>
+        <f>Discount!L33</f>
+        <v>GBP_YCRH_11YOIS#0000</v>
       </c>
       <c r="F62" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
@@ -4956,8 +4954,8 @@
         <v>37</v>
       </c>
       <c r="E63" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_12YOIS</v>
+        <f>Discount!L34</f>
+        <v>GBP_YCRH_12YOIS#0000</v>
       </c>
       <c r="F63" s="13">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
@@ -4988,25 +4986,25 @@
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B64" s="16"/>
       <c r="C64" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D64" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E64" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_13YOIS</v>
-      </c>
-      <c r="F64" s="13" t="e">
+        <f>Discount!L35</f>
+        <v>GBP_YCRH_15YOIS#0000</v>
+      </c>
+      <c r="F64" s="13">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.3949999999999999E-2</v>
       </c>
       <c r="G64" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E64,Trigger)</f>
         <v>#NUM!</v>
       </c>
       <c r="H64" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" s="12">
         <v>50</v>
@@ -5014,37 +5012,37 @@
       <c r="J64" s="12">
         <v>1</v>
       </c>
-      <c r="K64" s="11" t="e">
+      <c r="K64" s="11">
         <f>_xll.qlRateHelperEarliestDate($E64,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L64" s="10" t="e">
+        <v>41653</v>
+      </c>
+      <c r="L64" s="10">
         <f>_xll.qlRateHelperLatestDate($E64,Trigger)</f>
-        <v>#NUM!</v>
+        <v>47133</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B65" s="16"/>
       <c r="C65" s="15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D65" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E65" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_14YOIS</v>
-      </c>
-      <c r="F65" s="13" t="e">
+        <f>Discount!L36</f>
+        <v>GBP_YCRH_20YOIS#0000</v>
+      </c>
+      <c r="F65" s="13">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
-        <v>#NUM!</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="G65" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E65,Trigger)</f>
         <v>#NUM!</v>
       </c>
       <c r="H65" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" s="12">
         <v>50</v>
@@ -5052,30 +5050,30 @@
       <c r="J65" s="12">
         <v>1</v>
       </c>
-      <c r="K65" s="11" t="e">
+      <c r="K65" s="11">
         <f>_xll.qlRateHelperEarliestDate($E65,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L65" s="10" t="e">
+        <v>41653</v>
+      </c>
+      <c r="L65" s="10">
         <f>_xll.qlRateHelperLatestDate($E65,Trigger)</f>
-        <v>#NUM!</v>
+        <v>48960</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="16"/>
       <c r="C66" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>37</v>
       </c>
       <c r="E66" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_15YOIS</v>
+        <f>Discount!L37</f>
+        <v>GBP_YCRH_25YOIS#0000</v>
       </c>
       <c r="F66" s="13">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
-        <v>2.3949999999999999E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="G66" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E66,Trigger)</f>
@@ -5096,58 +5094,59 @@
       </c>
       <c r="L66" s="10">
         <f>_xll.qlRateHelperLatestDate($E66,Trigger)</f>
-        <v>47133</v>
+        <v>50784</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B67" s="16"/>
-      <c r="C67" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67" s="14" t="s">
+      <c r="B67" s="9"/>
+      <c r="C67" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E67" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_16YOIS</v>
-      </c>
-      <c r="F67" s="13" t="e">
+      <c r="E67" s="7" t="str">
+        <f>Discount!L38</f>
+        <v>GBP_YCRH_30YOIS#0000</v>
+      </c>
+      <c r="F67" s="6">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G67" s="13" t="e">
+        <v>2.9699999999999997E-2</v>
+      </c>
+      <c r="G67" s="6" t="e">
         <f>_xll.qlSwapRateHelperSpread($E67,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H67" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I67" s="12">
+      <c r="H67" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="5">
         <v>50</v>
       </c>
-      <c r="J67" s="12">
+      <c r="J67" s="5">
         <v>1</v>
       </c>
-      <c r="K67" s="11" t="e">
+      <c r="K67" s="4">
         <f>_xll.qlRateHelperEarliestDate($E67,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L67" s="10" t="e">
+        <v>41653</v>
+      </c>
+      <c r="L67" s="3">
         <f>_xll.qlRateHelperLatestDate($E67,Trigger)</f>
-        <v>#NUM!</v>
+        <v>52610</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="16"/>
-      <c r="C68" s="15" t="s">
-        <v>17</v>
+      <c r="C68" s="15" t="str">
+        <f t="shared" ref="C68:C104" si="3">IborType&amp;"BASIS"</f>
+        <v>OISBASIS</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E68" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_17YOIS</v>
+        <f t="shared" ref="E68:E73" si="4">RateHelperPrefix&amp;"_"&amp;$B68&amp;$C68&amp;$D68</f>
+        <v>GBP_YCRH_OISBASIS1Y</v>
       </c>
       <c r="F68" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
@@ -5161,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J68" s="12">
         <v>1</v>
@@ -5177,15 +5176,16 @@
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="16"/>
-      <c r="C69" s="15" t="s">
-        <v>16</v>
+      <c r="C69" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E69" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_18YOIS</v>
+        <f t="shared" si="4"/>
+        <v>GBP_YCRH_OISBASIS15M</v>
       </c>
       <c r="F69" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
@@ -5199,7 +5199,7 @@
         <v>0</v>
       </c>
       <c r="I69" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J69" s="12">
         <v>1</v>
@@ -5215,15 +5215,16 @@
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="16"/>
-      <c r="C70" s="15" t="s">
-        <v>15</v>
+      <c r="C70" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E70" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_19YOIS</v>
+        <f t="shared" si="4"/>
+        <v>GBP_YCRH_OISBASIS18M</v>
       </c>
       <c r="F70" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
@@ -5237,7 +5238,7 @@
         <v>0</v>
       </c>
       <c r="I70" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J70" s="12">
         <v>1</v>
@@ -5253,53 +5254,55 @@
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="16"/>
-      <c r="C71" s="15" t="s">
-        <v>14</v>
+      <c r="C71" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E71" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_20YOIS</v>
-      </c>
-      <c r="F71" s="13">
+        <f t="shared" si="4"/>
+        <v>GBP_YCRH_OISBASIS21M</v>
+      </c>
+      <c r="F71" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
-        <v>2.7099999999999999E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G71" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E71,Trigger)</f>
         <v>#NUM!</v>
       </c>
       <c r="H71" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J71" s="12">
         <v>1</v>
       </c>
-      <c r="K71" s="11">
+      <c r="K71" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E71,Trigger)</f>
-        <v>41653</v>
-      </c>
-      <c r="L71" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L71" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E71,Trigger)</f>
-        <v>48960</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="16"/>
-      <c r="C72" s="15" t="s">
-        <v>13</v>
+      <c r="C72" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E72" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_21YOIS</v>
+        <f t="shared" si="4"/>
+        <v>GBP_YCRH_OISBASIS2Y</v>
       </c>
       <c r="F72" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
@@ -5313,7 +5316,7 @@
         <v>0</v>
       </c>
       <c r="I72" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J72" s="12">
         <v>1</v>
@@ -5329,15 +5332,16 @@
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B73" s="16"/>
-      <c r="C73" s="15" t="s">
-        <v>12</v>
+      <c r="C73" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E73" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_22YOIS</v>
+        <f t="shared" si="4"/>
+        <v>GBP_YCRH_OISBASIS3Y</v>
       </c>
       <c r="F73" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
@@ -5351,7 +5355,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J73" s="12">
         <v>1</v>
@@ -5367,15 +5371,16 @@
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B74" s="16"/>
-      <c r="C74" s="15" t="s">
-        <v>11</v>
+      <c r="C74" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E74" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_23YOIS</v>
+        <f t="shared" ref="E74:E104" si="5">RateHelperPrefix&amp;"_"&amp;$B74&amp;$C74&amp;$D74</f>
+        <v>GBP_YCRH_OISBASIS4Y</v>
       </c>
       <c r="F74" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
@@ -5389,7 +5394,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J74" s="12">
         <v>1</v>
@@ -5405,15 +5410,16 @@
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B75" s="16"/>
-      <c r="C75" s="15" t="s">
-        <v>10</v>
+      <c r="C75" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E75" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_24YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS5Y</v>
       </c>
       <c r="F75" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
@@ -5427,7 +5433,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J75" s="12">
         <v>1</v>
@@ -5443,53 +5449,55 @@
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B76" s="16"/>
-      <c r="C76" s="15" t="s">
-        <v>9</v>
+      <c r="C76" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E76" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_25YOIS</v>
-      </c>
-      <c r="F76" s="13">
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS6Y</v>
+      </c>
+      <c r="F76" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
-        <v>2.8799999999999999E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G76" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E76,Trigger)</f>
         <v>#NUM!</v>
       </c>
       <c r="H76" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J76" s="12">
         <v>1</v>
       </c>
-      <c r="K76" s="11">
+      <c r="K76" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E76,Trigger)</f>
-        <v>41653</v>
-      </c>
-      <c r="L76" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L76" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E76,Trigger)</f>
-        <v>50784</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B77" s="16"/>
-      <c r="C77" s="15" t="s">
-        <v>8</v>
+      <c r="C77" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E77" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_26YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS7Y</v>
       </c>
       <c r="F77" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
@@ -5503,7 +5511,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J77" s="12">
         <v>1</v>
@@ -5519,15 +5527,16 @@
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B78" s="16"/>
-      <c r="C78" s="15" t="s">
-        <v>7</v>
+      <c r="C78" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="E78" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_27YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS8Y</v>
       </c>
       <c r="F78" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E78,Trigger)</f>
@@ -5541,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="I78" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J78" s="12">
         <v>1</v>
@@ -5557,15 +5566,16 @@
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B79" s="16"/>
-      <c r="C79" s="15" t="s">
-        <v>6</v>
+      <c r="C79" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E79" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_28YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS9Y</v>
       </c>
       <c r="F79" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E79,Trigger)</f>
@@ -5579,7 +5589,7 @@
         <v>0</v>
       </c>
       <c r="I79" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J79" s="12">
         <v>1</v>
@@ -5595,15 +5605,16 @@
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B80" s="16"/>
-      <c r="C80" s="15" t="s">
-        <v>5</v>
+      <c r="C80" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="E80" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_29YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS10Y</v>
       </c>
       <c r="F80" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E80,Trigger)</f>
@@ -5617,7 +5628,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J80" s="12">
         <v>1</v>
@@ -5633,53 +5644,55 @@
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B81" s="16"/>
-      <c r="C81" s="15" t="s">
-        <v>4</v>
+      <c r="C81" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E81" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_30YOIS</v>
-      </c>
-      <c r="F81" s="13">
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS11Y</v>
+      </c>
+      <c r="F81" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E81,Trigger)</f>
-        <v>2.9699999999999997E-2</v>
+        <v>#NUM!</v>
       </c>
       <c r="G81" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E81,Trigger)</f>
         <v>#NUM!</v>
       </c>
       <c r="H81" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J81" s="12">
         <v>1</v>
       </c>
-      <c r="K81" s="11">
+      <c r="K81" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41653</v>
-      </c>
-      <c r="L81" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L81" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>52610</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B82" s="16"/>
-      <c r="C82" s="15" t="s">
-        <v>3</v>
+      <c r="C82" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E82" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_35YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS12Y</v>
       </c>
       <c r="F82" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E82,Trigger)</f>
@@ -5693,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J82" s="12">
         <v>1</v>
@@ -5709,15 +5722,16 @@
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B83" s="16"/>
-      <c r="C83" s="15" t="s">
-        <v>2</v>
+      <c r="C83" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="E83" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_40YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS13Y</v>
       </c>
       <c r="F83" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E83,Trigger)</f>
@@ -5731,7 +5745,7 @@
         <v>0</v>
       </c>
       <c r="I83" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J83" s="12">
         <v>1</v>
@@ -5747,15 +5761,16 @@
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B84" s="16"/>
-      <c r="C84" s="15" t="s">
-        <v>1</v>
+      <c r="C84" s="15" t="str">
+        <f t="shared" si="3"/>
+        <v>OISBASIS</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E84" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_50YOIS</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS14Y</v>
       </c>
       <c r="F84" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
@@ -5769,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="12">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="J84" s="12">
         <v>1</v>
@@ -5784,39 +5799,40 @@
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B85" s="9"/>
-      <c r="C85" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E85" s="7" t="str">
+      <c r="B85" s="16"/>
+      <c r="C85" s="15" t="str">
         <f t="shared" si="3"/>
-        <v>GBP_YCRH_60YOIS</v>
-      </c>
-      <c r="F85" s="6" t="e">
+        <v>OISBASIS</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E85" s="14" t="str">
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS15Y</v>
+      </c>
+      <c r="F85" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G85" s="6" t="e">
+      <c r="G85" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E85,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="H85" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I85" s="5">
-        <v>50</v>
-      </c>
-      <c r="J85" s="5">
+      <c r="H85" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" s="12">
+        <v>40</v>
+      </c>
+      <c r="J85" s="12">
         <v>1</v>
       </c>
-      <c r="K85" s="4" t="e">
+      <c r="K85" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
         <v>#NUM!</v>
       </c>
-      <c r="L85" s="3" t="e">
+      <c r="L85" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
         <v>#NUM!</v>
       </c>
@@ -5824,15 +5840,15 @@
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B86" s="16"/>
       <c r="C86" s="15" t="str">
-        <f t="shared" ref="C86:C122" si="4">IborType&amp;"BASIS"</f>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E86" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_OISBASIS1Y</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS16Y</v>
       </c>
       <c r="F86" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E86,Trigger)</f>
@@ -5863,15 +5879,15 @@
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B87" s="16"/>
       <c r="C87" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E87" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_OISBASIS15M</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS17Y</v>
       </c>
       <c r="F87" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E87,Trigger)</f>
@@ -5902,15 +5918,15 @@
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B88" s="16"/>
       <c r="C88" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E88" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_OISBASIS18M</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS18Y</v>
       </c>
       <c r="F88" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E88,Trigger)</f>
@@ -5941,15 +5957,15 @@
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B89" s="16"/>
       <c r="C89" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E89" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_OISBASIS21M</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS19Y</v>
       </c>
       <c r="F89" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E89,Trigger)</f>
@@ -5980,15 +5996,15 @@
     <row r="90" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B90" s="16"/>
       <c r="C90" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E90" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_OISBASIS2Y</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS20Y</v>
       </c>
       <c r="F90" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E90,Trigger)</f>
@@ -6019,15 +6035,15 @@
     <row r="91" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B91" s="16"/>
       <c r="C91" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E91" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v>GBP_YCRH_OISBASIS3Y</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS21Y</v>
       </c>
       <c r="F91" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E91,Trigger)</f>
@@ -6058,15 +6074,15 @@
     <row r="92" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B92" s="16"/>
       <c r="C92" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E92" s="14" t="str">
-        <f t="shared" ref="E92:E122" si="5">RateHelperPrefix&amp;"_"&amp;$B92&amp;$C92&amp;$D92</f>
-        <v>GBP_YCRH_OISBASIS4Y</v>
+        <f t="shared" si="5"/>
+        <v>GBP_YCRH_OISBASIS22Y</v>
       </c>
       <c r="F92" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E92,Trigger)</f>
@@ -6097,15 +6113,15 @@
     <row r="93" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B93" s="16"/>
       <c r="C93" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E93" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS5Y</v>
+        <v>GBP_YCRH_OISBASIS23Y</v>
       </c>
       <c r="F93" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E93,Trigger)</f>
@@ -6136,15 +6152,15 @@
     <row r="94" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B94" s="16"/>
       <c r="C94" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E94" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS6Y</v>
+        <v>GBP_YCRH_OISBASIS24Y</v>
       </c>
       <c r="F94" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E94,Trigger)</f>
@@ -6175,15 +6191,15 @@
     <row r="95" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B95" s="16"/>
       <c r="C95" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E95" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS7Y</v>
+        <v>GBP_YCRH_OISBASIS25Y</v>
       </c>
       <c r="F95" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E95,Trigger)</f>
@@ -6214,15 +6230,15 @@
     <row r="96" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B96" s="16"/>
       <c r="C96" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E96" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS8Y</v>
+        <v>GBP_YCRH_OISBASIS26Y</v>
       </c>
       <c r="F96" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E96,Trigger)</f>
@@ -6253,15 +6269,15 @@
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B97" s="16"/>
       <c r="C97" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E97" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS9Y</v>
+        <v>GBP_YCRH_OISBASIS27Y</v>
       </c>
       <c r="F97" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E97,Trigger)</f>
@@ -6292,15 +6308,15 @@
     <row r="98" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B98" s="16"/>
       <c r="C98" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E98" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS10Y</v>
+        <v>GBP_YCRH_OISBASIS28Y</v>
       </c>
       <c r="F98" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E98,Trigger)</f>
@@ -6331,15 +6347,15 @@
     <row r="99" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B99" s="16"/>
       <c r="C99" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E99" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS11Y</v>
+        <v>GBP_YCRH_OISBASIS29Y</v>
       </c>
       <c r="F99" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E99,Trigger)</f>
@@ -6370,15 +6386,15 @@
     <row r="100" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B100" s="16"/>
       <c r="C100" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E100" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS12Y</v>
+        <v>GBP_YCRH_OISBASIS30Y</v>
       </c>
       <c r="F100" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E100,Trigger)</f>
@@ -6409,15 +6425,15 @@
     <row r="101" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B101" s="16"/>
       <c r="C101" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E101" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS13Y</v>
+        <v>GBP_YCRH_OISBASIS35Y</v>
       </c>
       <c r="F101" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E101,Trigger)</f>
@@ -6448,15 +6464,15 @@
     <row r="102" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B102" s="16"/>
       <c r="C102" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E102" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS14Y</v>
+        <v>GBP_YCRH_OISBASIS40Y</v>
       </c>
       <c r="F102" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E102,Trigger)</f>
@@ -6487,15 +6503,15 @@
     <row r="103" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B103" s="16"/>
       <c r="C103" s="15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E103" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS15Y</v>
+        <v>GBP_YCRH_OISBASIS50Y</v>
       </c>
       <c r="F103" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E103,Trigger)</f>
@@ -6524,743 +6540,41 @@
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B104" s="16"/>
-      <c r="C104" s="15" t="str">
-        <f t="shared" si="4"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="8" t="str">
+        <f t="shared" si="3"/>
         <v>OISBASIS</v>
       </c>
-      <c r="D104" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E104" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS16Y</v>
-      </c>
-      <c r="F104" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G104" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H104" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I104" s="12">
-        <v>40</v>
-      </c>
-      <c r="J104" s="12">
-        <v>1</v>
-      </c>
-      <c r="K104" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E104,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L104" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E104,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B105" s="16"/>
-      <c r="C105" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E105" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS17Y</v>
-      </c>
-      <c r="F105" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E105,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G105" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E105,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H105" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I105" s="12">
-        <v>40</v>
-      </c>
-      <c r="J105" s="12">
-        <v>1</v>
-      </c>
-      <c r="K105" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E105,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L105" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E105,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B106" s="16"/>
-      <c r="C106" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E106" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS18Y</v>
-      </c>
-      <c r="F106" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E106,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G106" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E106,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H106" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I106" s="12">
-        <v>40</v>
-      </c>
-      <c r="J106" s="12">
-        <v>1</v>
-      </c>
-      <c r="K106" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E106,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L106" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E106,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B107" s="16"/>
-      <c r="C107" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D107" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E107" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS19Y</v>
-      </c>
-      <c r="F107" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E107,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G107" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E107,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H107" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I107" s="12">
-        <v>40</v>
-      </c>
-      <c r="J107" s="12">
-        <v>1</v>
-      </c>
-      <c r="K107" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E107,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L107" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E107,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B108" s="16"/>
-      <c r="C108" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E108" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS20Y</v>
-      </c>
-      <c r="F108" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E108,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G108" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E108,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H108" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I108" s="12">
-        <v>40</v>
-      </c>
-      <c r="J108" s="12">
-        <v>1</v>
-      </c>
-      <c r="K108" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E108,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L108" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E108,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B109" s="16"/>
-      <c r="C109" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D109" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E109" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS21Y</v>
-      </c>
-      <c r="F109" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E109,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G109" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E109,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H109" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I109" s="12">
-        <v>40</v>
-      </c>
-      <c r="J109" s="12">
-        <v>1</v>
-      </c>
-      <c r="K109" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E109,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L109" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E109,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B110" s="16"/>
-      <c r="C110" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E110" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS22Y</v>
-      </c>
-      <c r="F110" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E110,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G110" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E110,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H110" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I110" s="12">
-        <v>40</v>
-      </c>
-      <c r="J110" s="12">
-        <v>1</v>
-      </c>
-      <c r="K110" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E110,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L110" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E110,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B111" s="16"/>
-      <c r="C111" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D111" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E111" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS23Y</v>
-      </c>
-      <c r="F111" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E111,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G111" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E111,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H111" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I111" s="12">
-        <v>40</v>
-      </c>
-      <c r="J111" s="12">
-        <v>1</v>
-      </c>
-      <c r="K111" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E111,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L111" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E111,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B112" s="16"/>
-      <c r="C112" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D112" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E112" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS24Y</v>
-      </c>
-      <c r="F112" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E112,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G112" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E112,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H112" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I112" s="12">
-        <v>40</v>
-      </c>
-      <c r="J112" s="12">
-        <v>1</v>
-      </c>
-      <c r="K112" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E112,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L112" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E112,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="113" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B113" s="16"/>
-      <c r="C113" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E113" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS25Y</v>
-      </c>
-      <c r="F113" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E113,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G113" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E113,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H113" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I113" s="12">
-        <v>40</v>
-      </c>
-      <c r="J113" s="12">
-        <v>1</v>
-      </c>
-      <c r="K113" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E113,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L113" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E113,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="114" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B114" s="16"/>
-      <c r="C114" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E114" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS26Y</v>
-      </c>
-      <c r="F114" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E114,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G114" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E114,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H114" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I114" s="12">
-        <v>40</v>
-      </c>
-      <c r="J114" s="12">
-        <v>1</v>
-      </c>
-      <c r="K114" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E114,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L114" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E114,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="115" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B115" s="16"/>
-      <c r="C115" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E115" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS27Y</v>
-      </c>
-      <c r="F115" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E115,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G115" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E115,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H115" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I115" s="12">
-        <v>40</v>
-      </c>
-      <c r="J115" s="12">
-        <v>1</v>
-      </c>
-      <c r="K115" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E115,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L115" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E115,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="116" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B116" s="16"/>
-      <c r="C116" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS28Y</v>
-      </c>
-      <c r="F116" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E116,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G116" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E116,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H116" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I116" s="12">
-        <v>40</v>
-      </c>
-      <c r="J116" s="12">
-        <v>1</v>
-      </c>
-      <c r="K116" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E116,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L116" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E116,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B117" s="16"/>
-      <c r="C117" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E117" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS29Y</v>
-      </c>
-      <c r="F117" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E117,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G117" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E117,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H117" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I117" s="12">
-        <v>40</v>
-      </c>
-      <c r="J117" s="12">
-        <v>1</v>
-      </c>
-      <c r="K117" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E117,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L117" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E117,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B118" s="16"/>
-      <c r="C118" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E118" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS30Y</v>
-      </c>
-      <c r="F118" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E118,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G118" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E118,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H118" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I118" s="12">
-        <v>40</v>
-      </c>
-      <c r="J118" s="12">
-        <v>1</v>
-      </c>
-      <c r="K118" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E118,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L118" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E118,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="119" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B119" s="16"/>
-      <c r="C119" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E119" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS35Y</v>
-      </c>
-      <c r="F119" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E119,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G119" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E119,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H119" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I119" s="12">
-        <v>40</v>
-      </c>
-      <c r="J119" s="12">
-        <v>1</v>
-      </c>
-      <c r="K119" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E119,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L119" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E119,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="120" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B120" s="16"/>
-      <c r="C120" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D120" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E120" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS40Y</v>
-      </c>
-      <c r="F120" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E120,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G120" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E120,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H120" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I120" s="12">
-        <v>40</v>
-      </c>
-      <c r="J120" s="12">
-        <v>1</v>
-      </c>
-      <c r="K120" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E120,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L120" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E120,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="121" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B121" s="16"/>
-      <c r="C121" s="15" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E121" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v>GBP_YCRH_OISBASIS50Y</v>
-      </c>
-      <c r="F121" s="13" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E121,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G121" s="13" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E121,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H121" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I121" s="12">
-        <v>40</v>
-      </c>
-      <c r="J121" s="12">
-        <v>1</v>
-      </c>
-      <c r="K121" s="11" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E121,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L121" s="10" t="e">
-        <f>_xll.qlRateHelperLatestDate($E121,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="122" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B122" s="9"/>
-      <c r="C122" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>OISBASIS</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E122" s="7" t="str">
+      <c r="D104" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="7" t="str">
         <f t="shared" si="5"/>
         <v>GBP_YCRH_OISBASIS60Y</v>
       </c>
-      <c r="F122" s="6" t="e">
-        <f>_xll.qlRateHelperQuoteValue($E122,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="G122" s="6" t="e">
-        <f>_xll.qlSwapRateHelperSpread($E122,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="H122" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I122" s="5">
+      <c r="F104" s="6" t="e">
+        <f>_xll.qlRateHelperQuoteValue($E104,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="G104" s="6" t="e">
+        <f>_xll.qlSwapRateHelperSpread($E104,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="H104" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I104" s="5">
         <v>40</v>
       </c>
-      <c r="J122" s="5">
+      <c r="J104" s="5">
         <v>1</v>
       </c>
-      <c r="K122" s="4" t="e">
-        <f>_xll.qlRateHelperEarliestDate($E122,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="L122" s="3" t="e">
-        <f>_xll.qlRateHelperLatestDate($E122,Trigger)</f>
+      <c r="K104" s="4" t="e">
+        <f>_xll.qlRateHelperEarliestDate($E104,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L104" s="3" t="e">
+        <f>_xll.qlRateHelperLatestDate($E104,Trigger)</f>
         <v>#NUM!</v>
       </c>
     </row>
@@ -7302,10 +6616,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="156" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="144"/>
+      <c r="B1" s="157"/>
       <c r="D1" s="52" t="s">
         <v>87</v>
       </c>
@@ -7525,7 +6839,7 @@
     <row r="7" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_RateHelpersSelected#0006</v>
+        <v>GBP_YCRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="42" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10701,7 +10015,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10723,7 +10039,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="140" t="s">
         <v>175</v>
       </c>
       <c r="B1" s="120"/>
@@ -10818,7 +10134,7 @@
       </c>
       <c r="L4" s="113" t="str">
         <f>_xll.qlEonia(K4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>GBP_YCRH__Libor#0007</v>
+        <v>GBP_YCRH__Libor#0000</v>
       </c>
       <c r="M4" s="112" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -10879,7 +10195,7 @@
       </c>
       <c r="L6" s="101" t="str">
         <f>_xll.qlOISRateHelper(K6,B6,C6,J6,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_SWOIS#0007</v>
+        <v>GBP_YCRH_SWOIS#0000</v>
       </c>
       <c r="M6" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -10933,7 +10249,7 @@
       </c>
       <c r="L7" s="101" t="str">
         <f>_xll.qlOISRateHelper(K7,B7,C7,J7,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_2WOIS#0007</v>
+        <v>GBP_YCRH_2WOIS#0000</v>
       </c>
       <c r="M7" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -10987,7 +10303,7 @@
       </c>
       <c r="L8" s="101" t="str">
         <f>_xll.qlOISRateHelper(K8,B8,C8,J8,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_3WOIS#0007</v>
+        <v>GBP_YCRH_3WOIS#0000</v>
       </c>
       <c r="M8" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -11041,7 +10357,7 @@
       </c>
       <c r="L9" s="101" t="str">
         <f>_xll.qlOISRateHelper(K9,B9,C9,J9,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_1MOIS#0007</v>
+        <v>GBP_YCRH_1MOIS#0000</v>
       </c>
       <c r="M9" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -11095,7 +10411,7 @@
       </c>
       <c r="L10" s="101" t="str">
         <f>_xll.qlOISRateHelper(K10,B10,C10,J10,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_2MOIS#0007</v>
+        <v>GBP_YCRH_2MOIS#0000</v>
       </c>
       <c r="M10" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -11149,7 +10465,7 @@
       </c>
       <c r="L11" s="101" t="str">
         <f>_xll.qlOISRateHelper(K11,B11,C11,J11,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_3MOIS#0007</v>
+        <v>GBP_YCRH_3MOIS#0000</v>
       </c>
       <c r="M11" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -11203,7 +10519,7 @@
       </c>
       <c r="L12" s="101" t="str">
         <f>_xll.qlOISRateHelper(K12,B12,C12,J12,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_4MOIS#0007</v>
+        <v>GBP_YCRH_4MOIS#0000</v>
       </c>
       <c r="M12" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -11257,7 +10573,7 @@
       </c>
       <c r="L13" s="101" t="str">
         <f>_xll.qlOISRateHelper(K13,B13,C13,J13,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_5MOIS#0007</v>
+        <v>GBP_YCRH_5MOIS#0000</v>
       </c>
       <c r="M13" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -11311,7 +10627,7 @@
       </c>
       <c r="L14" s="101" t="str">
         <f>_xll.qlOISRateHelper(K14,B14,C14,J14,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_6MOIS#0007</v>
+        <v>GBP_YCRH_6MOIS#0000</v>
       </c>
       <c r="M14" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -11365,7 +10681,7 @@
       </c>
       <c r="L15" s="101" t="str">
         <f>_xll.qlOISRateHelper(K15,B15,C15,J15,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_7MOIS#0007</v>
+        <v>GBP_YCRH_7MOIS#0000</v>
       </c>
       <c r="M15" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -11419,7 +10735,7 @@
       </c>
       <c r="L16" s="101" t="str">
         <f>_xll.qlOISRateHelper(K16,B16,C16,J16,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_8MOIS#0007</v>
+        <v>GBP_YCRH_8MOIS#0000</v>
       </c>
       <c r="M16" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -11473,7 +10789,7 @@
       </c>
       <c r="L17" s="101" t="str">
         <f>_xll.qlOISRateHelper(K17,B17,C17,J17,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_9MOIS#0007</v>
+        <v>GBP_YCRH_9MOIS#0000</v>
       </c>
       <c r="M17" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -11527,7 +10843,7 @@
       </c>
       <c r="L18" s="101" t="str">
         <f>_xll.qlOISRateHelper(K18,B18,C18,J18,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_10MOIS#0007</v>
+        <v>GBP_YCRH_10MOIS#0000</v>
       </c>
       <c r="M18" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -11581,7 +10897,7 @@
       </c>
       <c r="L19" s="101" t="str">
         <f>_xll.qlOISRateHelper(K19,B19,C19,J19,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_11MOIS#0007</v>
+        <v>GBP_YCRH_11MOIS#0000</v>
       </c>
       <c r="M19" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -11635,7 +10951,7 @@
       </c>
       <c r="L20" s="101" t="str">
         <f>_xll.qlOISRateHelper(K20,B20,C20,J20,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_1YOIS#0007</v>
+        <v>GBP_YCRH_1YOIS#0000</v>
       </c>
       <c r="M20" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -11689,7 +11005,7 @@
       </c>
       <c r="L21" s="101" t="str">
         <f>_xll.qlOISRateHelper(K21,B21,C21,J21,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_15MOIS#0007</v>
+        <v>GBP_YCRH_15MOIS#0000</v>
       </c>
       <c r="M21" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -11743,7 +11059,7 @@
       </c>
       <c r="L22" s="101" t="str">
         <f>_xll.qlOISRateHelper(K22,B22,C22,J22,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_18MOIS#0007</v>
+        <v>GBP_YCRH_18MOIS#0000</v>
       </c>
       <c r="M22" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -11797,7 +11113,7 @@
       </c>
       <c r="L23" s="101" t="str">
         <f>_xll.qlOISRateHelper(K23,B23,C23,J23,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_21MOIS#0007</v>
+        <v>GBP_YCRH_21MOIS#0000</v>
       </c>
       <c r="M23" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -11851,7 +11167,7 @@
       </c>
       <c r="L24" s="101" t="str">
         <f>_xll.qlOISRateHelper(K24,B24,C24,J24,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_2YOIS#0007</v>
+        <v>GBP_YCRH_2YOIS#0000</v>
       </c>
       <c r="M24" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -11905,7 +11221,7 @@
       </c>
       <c r="L25" s="101" t="str">
         <f>_xll.qlOISRateHelper(K25,B25,C25,J25,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_3YOIS#0007</v>
+        <v>GBP_YCRH_3YOIS#0000</v>
       </c>
       <c r="M25" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -11959,7 +11275,7 @@
       </c>
       <c r="L26" s="101" t="str">
         <f>_xll.qlOISRateHelper(K26,B26,C26,J26,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_4YOIS#0007</v>
+        <v>GBP_YCRH_4YOIS#0000</v>
       </c>
       <c r="M26" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -12013,7 +11329,7 @@
       </c>
       <c r="L27" s="101" t="str">
         <f>_xll.qlOISRateHelper(K27,B27,C27,J27,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_5YOIS#0007</v>
+        <v>GBP_YCRH_5YOIS#0000</v>
       </c>
       <c r="M27" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -12067,7 +11383,7 @@
       </c>
       <c r="L28" s="101" t="str">
         <f>_xll.qlOISRateHelper(K28,B28,C28,J28,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_6YOIS#0007</v>
+        <v>GBP_YCRH_6YOIS#0000</v>
       </c>
       <c r="M28" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -12121,7 +11437,7 @@
       </c>
       <c r="L29" s="101" t="str">
         <f>_xll.qlOISRateHelper(K29,B29,C29,J29,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_7YOIS#0007</v>
+        <v>GBP_YCRH_7YOIS#0000</v>
       </c>
       <c r="M29" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -12175,7 +11491,7 @@
       </c>
       <c r="L30" s="101" t="str">
         <f>_xll.qlOISRateHelper(K30,B30,C30,J30,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_8YOIS#0007</v>
+        <v>GBP_YCRH_8YOIS#0000</v>
       </c>
       <c r="M30" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -12229,7 +11545,7 @@
       </c>
       <c r="L31" s="101" t="str">
         <f>_xll.qlOISRateHelper(K31,B31,C31,J31,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_9YOIS#0007</v>
+        <v>GBP_YCRH_9YOIS#0000</v>
       </c>
       <c r="M31" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -12283,7 +11599,7 @@
       </c>
       <c r="L32" s="101" t="str">
         <f>_xll.qlOISRateHelper(K32,B32,C32,J32,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_10YOIS#0007</v>
+        <v>GBP_YCRH_10YOIS#0000</v>
       </c>
       <c r="M32" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -12337,7 +11653,7 @@
       </c>
       <c r="L33" s="101" t="str">
         <f>_xll.qlOISRateHelper(K33,B33,C33,J33,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_11YOIS#0007</v>
+        <v>GBP_YCRH_11YOIS#0000</v>
       </c>
       <c r="M33" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -12391,7 +11707,7 @@
       </c>
       <c r="L34" s="101" t="str">
         <f>_xll.qlOISRateHelper(K34,B34,C34,J34,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_12YOIS#0007</v>
+        <v>GBP_YCRH_12YOIS#0000</v>
       </c>
       <c r="M34" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -12445,7 +11761,7 @@
       </c>
       <c r="L35" s="101" t="str">
         <f>_xll.qlOISRateHelper(K35,B35,C35,J35,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_15YOIS#0007</v>
+        <v>GBP_YCRH_15YOIS#0000</v>
       </c>
       <c r="M35" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -12499,7 +11815,7 @@
       </c>
       <c r="L36" s="101" t="str">
         <f>_xll.qlOISRateHelper(K36,B36,C36,J36,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_20YOIS#0007</v>
+        <v>GBP_YCRH_20YOIS#0000</v>
       </c>
       <c r="M36" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -12553,7 +11869,7 @@
       </c>
       <c r="L37" s="101" t="str">
         <f>_xll.qlOISRateHelper(K37,B37,C37,J37,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_25YOIS#0007</v>
+        <v>GBP_YCRH_25YOIS#0000</v>
       </c>
       <c r="M37" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -12607,7 +11923,7 @@
       </c>
       <c r="L38" s="101" t="str">
         <f>_xll.qlOISRateHelper(K38,B38,C38,J38,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_30YOIS#0007</v>
+        <v>GBP_YCRH_30YOIS#0000</v>
       </c>
       <c r="M38" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -12679,7 +11995,7 @@
       </c>
       <c r="L40" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K40,B40,B41,J40,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCJAN11OIS#0007</v>
+        <v>GBP_YCRH_MPCJAN11OIS#0000</v>
       </c>
       <c r="M40" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -12733,7 +12049,7 @@
       </c>
       <c r="L41" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K41,B41,B42,J41,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCFEB11OIS#0007</v>
+        <v>GBP_YCRH_MPCFEB11OIS#0000</v>
       </c>
       <c r="M41" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -12787,7 +12103,7 @@
       </c>
       <c r="L42" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K42,B42,B43,J42,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCMAR11OIS#0007</v>
+        <v>GBP_YCRH_MPCMAR11OIS#0000</v>
       </c>
       <c r="M42" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -12841,7 +12157,7 @@
       </c>
       <c r="L43" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K43,B43,B44,J43,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCAPR11OIS#0007</v>
+        <v>GBP_YCRH_MPCAPR11OIS#0000</v>
       </c>
       <c r="M43" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L43)</f>
@@ -12895,7 +12211,7 @@
       </c>
       <c r="L44" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K44,B44,B45,J44,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCMAY11OIS#0007</v>
+        <v>GBP_YCRH_MPCMAY11OIS#0000</v>
       </c>
       <c r="M44" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -12949,7 +12265,7 @@
       </c>
       <c r="L45" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K45,B45,B46,J45,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCJUN11OIS#0007</v>
+        <v>GBP_YCRH_MPCJUN11OIS#0000</v>
       </c>
       <c r="M45" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -13003,7 +12319,7 @@
       </c>
       <c r="L46" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K46,B46,B47,J46,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCJUL11OIS#0007</v>
+        <v>GBP_YCRH_MPCJUL11OIS#0000</v>
       </c>
       <c r="M46" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -13057,7 +12373,7 @@
       </c>
       <c r="L47" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K47,B47,B48,J47,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCAUG11OIS#0007</v>
+        <v>GBP_YCRH_MPCAUG11OIS#0000</v>
       </c>
       <c r="M47" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -13111,7 +12427,7 @@
       </c>
       <c r="L48" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K48,B48,B49,J48,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCSEP11OIS#0007</v>
+        <v>GBP_YCRH_MPCSEP11OIS#0000</v>
       </c>
       <c r="M48" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -13165,7 +12481,7 @@
       </c>
       <c r="L49" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K49,B49,B50,J49,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCOCT11OIS#0007</v>
+        <v>GBP_YCRH_MPCOCT11OIS#0000</v>
       </c>
       <c r="M49" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -13219,7 +12535,7 @@
       </c>
       <c r="L50" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K50,B50,B51,J50,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCNOV11OIS#0007</v>
+        <v>GBP_YCRH_MPCNOV11OIS#0000</v>
       </c>
       <c r="M50" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -13273,7 +12589,7 @@
       </c>
       <c r="L51" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K51,B51,B52,J51,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCDEC11OIS#0007</v>
+        <v>GBP_YCRH_MPCDEC11OIS#0000</v>
       </c>
       <c r="M51" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L51)</f>
@@ -13327,7 +12643,7 @@
       </c>
       <c r="L52" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K52,B52,B53,J52,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCJAN12OIS#0007</v>
+        <v>GBP_YCRH_MPCJAN12OIS#0000</v>
       </c>
       <c r="M52" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L52)</f>
@@ -13381,7 +12697,7 @@
       </c>
       <c r="L53" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K53,B53,B54,J53,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCFEB12OIS#0007</v>
+        <v>GBP_YCRH_MPCFEB12OIS#0000</v>
       </c>
       <c r="M53" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L53)</f>
@@ -13435,7 +12751,7 @@
       </c>
       <c r="L54" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K54,B54,B55,J54,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCMAR12OIS#0007</v>
+        <v>GBP_YCRH_MPCMAR12OIS#0000</v>
       </c>
       <c r="M54" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L54)</f>
@@ -13489,7 +12805,7 @@
       </c>
       <c r="L55" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K55,B55,B56,J55,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCAPR12OIS#0007</v>
+        <v>GBP_YCRH_MPCAPR12OIS#0000</v>
       </c>
       <c r="M55" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L55)</f>
@@ -13543,7 +12859,7 @@
       </c>
       <c r="L56" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K56,B56,B57,J56,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCMAY12OIS#0007</v>
+        <v>GBP_YCRH_MPCMAY12OIS#0000</v>
       </c>
       <c r="M56" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L56)</f>
@@ -13597,7 +12913,7 @@
       </c>
       <c r="L57" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K57,B57,B58,J57,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCJUN12OIS#0007</v>
+        <v>GBP_YCRH_MPCJUN12OIS#0000</v>
       </c>
       <c r="M57" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L57)</f>
@@ -13651,7 +12967,7 @@
       </c>
       <c r="L58" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K58,B58,B59,J58,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCJUL12OIS#0007</v>
+        <v>GBP_YCRH_MPCJUL12OIS#0000</v>
       </c>
       <c r="M58" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L58)</f>
@@ -13705,7 +13021,7 @@
       </c>
       <c r="L59" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K59,B59,B60,J59,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCAUG12OIS#0007</v>
+        <v>GBP_YCRH_MPCAUG12OIS#0000</v>
       </c>
       <c r="M59" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L59)</f>
@@ -13759,7 +13075,7 @@
       </c>
       <c r="L60" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K60,B60,B61,J60,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCSEP12OIS#0007</v>
+        <v>GBP_YCRH_MPCSEP12OIS#0000</v>
       </c>
       <c r="M60" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L60)</f>
@@ -13813,7 +13129,7 @@
       </c>
       <c r="L61" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K61,B61,B62,J61,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCOCT12OIS#0007</v>
+        <v>GBP_YCRH_MPCOCT12OIS#0000</v>
       </c>
       <c r="M61" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L61)</f>
@@ -13867,7 +13183,7 @@
       </c>
       <c r="L62" s="101" t="str">
         <f>_xll.qlDatedOISRateHelper(K62,B62,B63,J62,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>GBP_YCRH_MPCNOV12OIS#0007</v>
+        <v>GBP_YCRH_MPCNOV12OIS#0000</v>
       </c>
       <c r="M62" s="108" t="str">
         <f>_xll.ohRangeRetrieveError(L62)</f>
@@ -13925,7 +13241,7 @@
       </c>
       <c r="M63" s="108" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L63)</f>
-        <v>qlDatedOISRateHelper - Error converting parameter 'EndDate' : 'unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'QuantLib::Date'</v>
+        <v/>
       </c>
       <c r="N63" s="96"/>
       <c r="P63" s="99" t="e">
@@ -13974,7 +13290,7 @@
       </c>
       <c r="M64" s="108" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L64)</f>
-        <v>qlDatedOISRateHelper - Error converting parameter 'StartDate' : 'unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'QuantLib::Date'</v>
+        <v/>
       </c>
       <c r="N64" s="96"/>
       <c r="P64" s="99" t="e">

</xml_diff>